<commit_message>
Updates to control files
</commit_message>
<xml_diff>
--- a/data/experiment_parameters.xlsx
+++ b/data/experiment_parameters.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -37,12 +37,27 @@
     <t>General</t>
   </si>
   <si>
+    <t>MODE</t>
+  </si>
+  <si>
+    <t>test</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>test or live</t>
+  </si>
+  <si>
+    <t>TRIAL_SLEEP_TIME</t>
+  </si>
+  <si>
+    <t>seconds</t>
+  </si>
+  <si>
     <t>SYSTEM_READY_SOUND_DURATION</t>
   </si>
   <si>
-    <t>seconds</t>
-  </si>
-  <si>
     <t>SESSION_STARTED_SOUND_DURATION</t>
   </si>
   <si>
@@ -52,10 +67,7 @@
     <t>N_SUBJECT</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
-    <t>N_TRIAL</t>
+    <t>TRIAL_LIMIT</t>
   </si>
   <si>
     <t>MAX_TRIAL_PER_SESSION</t>
@@ -121,7 +133,19 @@
     <t>pellets</t>
   </si>
   <si>
-    <t>Pellets or grain</t>
+    <t>pellets or grain</t>
+  </si>
+  <si>
+    <t>RP-H</t>
+  </si>
+  <si>
+    <t>RESPONSE_TIMEOUT</t>
+  </si>
+  <si>
+    <t>CRITERION_LIMIT_RP_H</t>
+  </si>
+  <si>
+    <t>CRITERION_TIME_RP_H</t>
   </si>
 </sst>
 </file>
@@ -452,26 +476,28 @@
       <c r="A3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4">
-        <v>1.0</v>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="4" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B4" s="4">
-        <v>1.0</v>
+        <v>5.0</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
@@ -480,13 +506,13 @@
     </row>
     <row r="5">
       <c r="A5" s="4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B5" s="4">
         <v>1.0</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -495,51 +521,43 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B6" s="4">
-        <v>20.0</v>
+        <v>1.0</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="4">
-        <v>10.0</v>
-      </c>
-      <c r="E6" s="4">
-        <v>30.0</v>
-      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="4"/>
     </row>
     <row r="7">
       <c r="A7" s="4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B7" s="4">
-        <v>10.0</v>
+        <v>1.0</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="E7" s="4">
-        <v>50.0</v>
-      </c>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
     <row r="8">
       <c r="A8" s="4" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" s="4">
         <v>20.0</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D8" s="4">
         <v>10.0</v>
@@ -547,242 +565,324 @@
       <c r="E8" s="4">
         <v>30.0</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
-      </c>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9">
       <c r="A9" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="E9" s="4">
+        <v>50.0</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="5">
         <f>5*60</f>
         <v>300</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4">
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" s="4">
         <v>0.0</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E11" s="5">
         <f>10*60</f>
         <v>600</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="4">
-        <v>10.0</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>20.0</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="6"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="4" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B12" s="4">
-        <v>3.0</v>
-      </c>
+        <v>10.0</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E12" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" s="4">
-        <v>5.0</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="E13" s="4">
-        <v>6.0</v>
-      </c>
+      <c r="A13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
     </row>
     <row r="14">
       <c r="A14" s="4" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B14" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E14" s="4">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
+      <c r="A15" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="E15" s="4">
+        <v>6.0</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="4" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B16" s="4">
-        <v>1.0</v>
+        <v>0.1</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="4">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E16" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G16" s="4" t="s">
-        <v>27</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B17" s="4">
-        <v>180.0</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="A17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="4">
-        <v>180.0</v>
-      </c>
-      <c r="E17" s="4">
-        <v>180.0</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>27</v>
-      </c>
+      <c r="B17" s="6"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
     </row>
     <row r="18">
       <c r="A18" s="4" t="s">
         <v>30</v>
       </c>
       <c r="B18" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D18" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="E18" s="4">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4">
+        <v>180.0</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="4">
+        <v>180.0</v>
+      </c>
+      <c r="E19" s="4">
+        <v>180.0</v>
+      </c>
+      <c r="G19" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B19" s="4">
-        <v>0.7</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="E19" s="4">
-        <v>2.0</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B20" s="4">
-        <v>3.0</v>
+        <v>0.0</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D20" s="4">
         <v>0.0</v>
       </c>
       <c r="E20" s="4">
-        <v>6.0</v>
+        <v>0.0</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="4" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B21" s="4">
-        <v>20.0</v>
+        <v>0.7</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="D21" s="4">
-        <v>10.0</v>
+        <v>0.0</v>
       </c>
       <c r="E21" s="4">
-        <v>50.0</v>
+        <v>2.0</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="B22" s="4">
+        <v>3.0</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G22" s="4" t="s">
-        <v>36</v>
+      <c r="D22" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="E22" s="4">
+        <v>6.0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D23" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="E23" s="4">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="6"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B26" s="4">
+        <v>45.0</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B27" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B28" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>